<commit_message>
EPBDS-12252 No link and hints is displayed for methods called in rule with merged condition
</commit_message>
<xml_diff>
--- a/DEV/org.openl.rules/test/rules/binding/MethodUsagesMetaInfoTest.xlsx
+++ b/DEV/org.openl.rules/test/rules/binding/MethodUsagesMetaInfoTest.xlsx
@@ -1,10 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="9302"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="24931"/>
   <workbookPr/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Projects\openl-tablets\DEV\org.openl.rules\test\rules\binding\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B13B32BB-84C7-4C8E-A22C-AA2AC19FDBAD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="285" yWindow="105" windowWidth="16140" windowHeight="9210"/>
+    <workbookView xWindow="10070" yWindow="8450" windowWidth="23600" windowHeight="12560" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Test" sheetId="5" r:id="rId1"/>
@@ -21,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="63" uniqueCount="49">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="113" uniqueCount="61">
   <si>
     <t>C1</t>
   </si>
@@ -172,11 +178,47 @@
   <si>
     <t>lob</t>
   </si>
+  <si>
+    <t>MC1</t>
+  </si>
+  <si>
+    <t>int</t>
+  </si>
+  <si>
+    <t>Cod1</t>
+  </si>
+  <si>
+    <t>Result</t>
+  </si>
+  <si>
+    <t>String[][]</t>
+  </si>
+  <si>
+    <t>String[]</t>
+  </si>
+  <si>
+    <t>= testDT(x)</t>
+  </si>
+  <si>
+    <t>x</t>
+  </si>
+  <si>
+    <t>Rules String[] testDT1(int x)</t>
+  </si>
+  <si>
+    <t>Rules String[][] testDT3(int x)</t>
+  </si>
+  <si>
+    <t>Rules String[] testDT2(int x)</t>
+  </si>
+  <si>
+    <t>Rules String[][] testDT4(int x)</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="9" x14ac:knownFonts="1">
     <font>
       <sz val="10"/>
@@ -377,7 +419,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="25">
+  <borders count="34">
     <border>
       <left/>
       <right/>
@@ -701,11 +743,116 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="64">
+  <cellXfs count="76">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
@@ -759,6 +906,9 @@
     <xf numFmtId="0" fontId="4" fillId="13" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="22" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="8" fillId="18" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -777,6 +927,46 @@
     <xf numFmtId="0" fontId="3" fillId="19" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="22" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="16" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="17" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="21" xfId="0" quotePrefix="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" quotePrefix="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="14" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="14" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="15" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="15" borderId="13" xfId="0" quotePrefix="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="23" borderId="22" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="23" borderId="23" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="23" borderId="24" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
     <xf numFmtId="0" fontId="6" fillId="20" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
@@ -801,48 +991,41 @@
     <xf numFmtId="0" fontId="1" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="21" xfId="0" quotePrefix="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" quotePrefix="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="16" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="17" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="14" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="14" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="15" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="15" borderId="13" xfId="0" quotePrefix="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="23" borderId="22" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="23" borderId="23" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="23" borderId="24" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="22" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="22" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="28" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="23" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="24" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="29" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="31" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="25" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="27" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="30" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="26" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="32" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="33" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -853,6 +1036,9 @@
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
     </ext>
   </extLst>
 </styleSheet>
@@ -1205,50 +1391,50 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="B3:M37"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <dimension ref="B3:M82"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C15" sqref="C15:D15"/>
+    <sheetView tabSelected="1" topLeftCell="A61" workbookViewId="0">
+      <selection activeCell="G71" sqref="G71"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultRowHeight="12.5" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="2" max="2" width="19.140625" customWidth="1"/>
-    <col min="3" max="3" width="23.42578125" customWidth="1"/>
-    <col min="4" max="4" width="13.7109375" customWidth="1"/>
-    <col min="5" max="5" width="12.42578125" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="28.140625" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="18.42578125" customWidth="1"/>
+    <col min="2" max="2" width="19.1796875" customWidth="1"/>
+    <col min="3" max="3" width="23.453125" customWidth="1"/>
+    <col min="4" max="4" width="13.7265625" customWidth="1"/>
+    <col min="5" max="5" width="12.453125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="28.1796875" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="18.453125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="3" spans="2:13" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B3" s="60" t="s">
+    <row r="3" spans="2:13" ht="13" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B3" s="35" t="s">
         <v>31</v>
       </c>
-      <c r="C3" s="60" t="s">
+      <c r="C3" s="35" t="s">
         <v>1</v>
       </c>
-      <c r="K3" s="35" t="s">
+      <c r="K3" s="36" t="s">
         <v>8</v>
       </c>
-      <c r="L3" s="36"/>
-      <c r="M3" s="37"/>
-    </row>
-    <row r="4" spans="2:13" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="L3" s="37"/>
+      <c r="M3" s="38"/>
+    </row>
+    <row r="4" spans="2:13" ht="13.5" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B4" s="5" t="s">
         <v>0</v>
       </c>
       <c r="C4" s="4" t="s">
         <v>3</v>
       </c>
-      <c r="K4" s="38" t="s">
+      <c r="K4" s="39" t="s">
         <v>4</v>
       </c>
-      <c r="L4" s="39"/>
-      <c r="M4" s="40"/>
-    </row>
-    <row r="5" spans="2:13" x14ac:dyDescent="0.2">
+      <c r="L4" s="40"/>
+      <c r="M4" s="41"/>
+    </row>
+    <row r="5" spans="2:13" x14ac:dyDescent="0.25">
       <c r="B5" s="3" t="s">
         <v>7</v>
       </c>
@@ -1256,7 +1442,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="6" spans="2:13" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="6" spans="2:13" ht="13" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B6" s="2" t="s">
         <v>11</v>
       </c>
@@ -1264,7 +1450,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="7" spans="2:13" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="7" spans="2:13" ht="13.5" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B7" s="6" t="s">
         <v>12</v>
       </c>
@@ -1272,60 +1458,60 @@
         <v>2</v>
       </c>
     </row>
-    <row r="8" spans="2:13" x14ac:dyDescent="0.2">
+    <row r="8" spans="2:13" x14ac:dyDescent="0.25">
       <c r="B8" s="7">
         <v>0</v>
       </c>
       <c r="C8" s="11" t="s">
         <v>9</v>
       </c>
-      <c r="K8" s="35" t="s">
+      <c r="K8" s="36" t="s">
         <v>37</v>
       </c>
-      <c r="L8" s="36"/>
-      <c r="M8" s="37"/>
-    </row>
-    <row r="9" spans="2:13" x14ac:dyDescent="0.2">
+      <c r="L8" s="37"/>
+      <c r="M8" s="38"/>
+    </row>
+    <row r="9" spans="2:13" x14ac:dyDescent="0.25">
       <c r="B9" s="8">
         <v>1</v>
       </c>
       <c r="C9" s="10" t="s">
         <v>10</v>
       </c>
-      <c r="K9" s="38" t="s">
+      <c r="K9" s="39" t="s">
         <v>36</v>
       </c>
-      <c r="L9" s="39"/>
-      <c r="M9" s="40"/>
-    </row>
-    <row r="10" spans="2:13" x14ac:dyDescent="0.2">
-      <c r="K10" s="38" t="s">
+      <c r="L9" s="40"/>
+      <c r="M9" s="41"/>
+    </row>
+    <row r="10" spans="2:13" x14ac:dyDescent="0.25">
+      <c r="K10" s="39" t="s">
         <v>43</v>
       </c>
-      <c r="L10" s="39"/>
-      <c r="M10" s="40"/>
-    </row>
-    <row r="11" spans="2:13" ht="48.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="K11" s="38" t="s">
+      <c r="L10" s="40"/>
+      <c r="M10" s="41"/>
+    </row>
+    <row r="11" spans="2:13" ht="48.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="K11" s="39" t="s">
         <v>45</v>
       </c>
-      <c r="L11" s="39"/>
-      <c r="M11" s="40"/>
-    </row>
-    <row r="12" spans="2:13" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B12" s="62" t="s">
+      <c r="L11" s="40"/>
+      <c r="M11" s="41"/>
+    </row>
+    <row r="12" spans="2:13" ht="13" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B12" s="43" t="s">
         <v>31</v>
       </c>
-      <c r="C12" s="62"/>
-      <c r="D12" s="62"/>
-      <c r="K12" s="38" t="s">
+      <c r="C12" s="43"/>
+      <c r="D12" s="43"/>
+      <c r="K12" s="39" t="s">
         <v>44</v>
       </c>
-      <c r="L12" s="39"/>
-      <c r="M12" s="40"/>
-    </row>
-    <row r="13" spans="2:13" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B13" s="61" t="s">
+      <c r="L12" s="40"/>
+      <c r="M12" s="41"/>
+    </row>
+    <row r="13" spans="2:13" ht="13.5" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B13" s="42" t="s">
         <v>38</v>
       </c>
       <c r="C13" s="5" t="s">
@@ -1335,8 +1521,8 @@
         <v>40647</v>
       </c>
     </row>
-    <row r="14" spans="2:13" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B14" s="61"/>
+    <row r="14" spans="2:13" ht="13.5" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B14" s="42"/>
       <c r="C14" s="5" t="s">
         <v>48</v>
       </c>
@@ -1344,70 +1530,70 @@
         <v>47</v>
       </c>
     </row>
-    <row r="15" spans="2:13" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="15" spans="2:13" ht="13.5" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B15" s="5" t="s">
         <v>0</v>
       </c>
-      <c r="C15" s="43" t="s">
+      <c r="C15" s="58" t="s">
         <v>3</v>
       </c>
-      <c r="D15" s="44"/>
-    </row>
-    <row r="16" spans="2:13" x14ac:dyDescent="0.2">
+      <c r="D15" s="59"/>
+    </row>
+    <row r="16" spans="2:13" x14ac:dyDescent="0.25">
       <c r="B16" s="3" t="s">
         <v>7</v>
       </c>
-      <c r="C16" s="45" t="s">
+      <c r="C16" s="60" t="s">
         <v>6</v>
       </c>
-      <c r="D16" s="46"/>
-    </row>
-    <row r="17" spans="2:6" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="D16" s="61"/>
+    </row>
+    <row r="17" spans="2:6" ht="13" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B17" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="C17" s="45" t="s">
+      <c r="C17" s="60" t="s">
         <v>5</v>
       </c>
-      <c r="D17" s="46"/>
-    </row>
-    <row r="18" spans="2:6" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="D17" s="61"/>
+    </row>
+    <row r="18" spans="2:6" ht="13.5" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B18" s="6" t="s">
         <v>12</v>
       </c>
-      <c r="C18" s="47" t="s">
+      <c r="C18" s="62" t="s">
         <v>2</v>
       </c>
-      <c r="D18" s="48"/>
-    </row>
-    <row r="19" spans="2:6" x14ac:dyDescent="0.2">
+      <c r="D18" s="63"/>
+    </row>
+    <row r="19" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B19" s="7">
         <v>0</v>
       </c>
-      <c r="C19" s="49" t="s">
+      <c r="C19" s="46" t="s">
         <v>40</v>
       </c>
-      <c r="D19" s="50"/>
-    </row>
-    <row r="20" spans="2:6" x14ac:dyDescent="0.2">
+      <c r="D19" s="47"/>
+    </row>
+    <row r="20" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B20" s="8">
         <v>1</v>
       </c>
-      <c r="C20" s="49" t="s">
+      <c r="C20" s="46" t="s">
         <v>41</v>
       </c>
-      <c r="D20" s="50"/>
-    </row>
-    <row r="23" spans="2:6" ht="15" x14ac:dyDescent="0.25">
-      <c r="B23" s="63" t="s">
+      <c r="D20" s="47"/>
+    </row>
+    <row r="23" spans="2:6" ht="14" x14ac:dyDescent="0.3">
+      <c r="B23" s="55" t="s">
         <v>26</v>
       </c>
-      <c r="C23" s="63"/>
-      <c r="D23" s="63"/>
-      <c r="E23" s="63"/>
-      <c r="F23" s="63"/>
-    </row>
-    <row r="24" spans="2:6" ht="14.25" x14ac:dyDescent="0.2">
+      <c r="C23" s="55"/>
+      <c r="D23" s="55"/>
+      <c r="E23" s="55"/>
+      <c r="F23" s="55"/>
+    </row>
+    <row r="24" spans="2:6" ht="14" x14ac:dyDescent="0.3">
       <c r="B24" s="14" t="s">
         <v>14</v>
       </c>
@@ -1424,25 +1610,25 @@
         <v>18</v>
       </c>
     </row>
-    <row r="25" spans="2:6" ht="14.25" x14ac:dyDescent="0.2">
-      <c r="B25" s="51" t="s">
+    <row r="25" spans="2:6" ht="14" x14ac:dyDescent="0.3">
+      <c r="B25" s="44" t="s">
         <v>19</v>
       </c>
-      <c r="C25" s="52" t="s">
+      <c r="C25" s="45" t="s">
         <v>15</v>
       </c>
-      <c r="D25" s="41" t="s">
+      <c r="D25" s="56" t="s">
         <v>16</v>
       </c>
-      <c r="E25" s="42" t="s">
+      <c r="E25" s="57" t="s">
         <v>20</v>
       </c>
-      <c r="F25" s="42"/>
-    </row>
-    <row r="26" spans="2:6" ht="14.25" x14ac:dyDescent="0.2">
-      <c r="B26" s="51"/>
-      <c r="C26" s="52"/>
-      <c r="D26" s="41"/>
+      <c r="F25" s="57"/>
+    </row>
+    <row r="26" spans="2:6" ht="14" x14ac:dyDescent="0.3">
+      <c r="B26" s="44"/>
+      <c r="C26" s="45"/>
+      <c r="D26" s="56"/>
       <c r="E26" s="19" t="s">
         <v>17</v>
       </c>
@@ -1450,7 +1636,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="27" spans="2:6" ht="15" x14ac:dyDescent="0.25">
+    <row r="27" spans="2:6" ht="14" x14ac:dyDescent="0.3">
       <c r="B27" s="21"/>
       <c r="C27" s="22" t="s">
         <v>21</v>
@@ -1465,7 +1651,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="28" spans="2:6" ht="15" x14ac:dyDescent="0.25">
+    <row r="28" spans="2:6" ht="14" x14ac:dyDescent="0.3">
       <c r="B28" s="21"/>
       <c r="C28" s="22"/>
       <c r="D28" s="21" t="s">
@@ -1478,7 +1664,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="29" spans="2:6" ht="15" x14ac:dyDescent="0.25">
+    <row r="29" spans="2:6" ht="14" x14ac:dyDescent="0.3">
       <c r="B29" s="21"/>
       <c r="C29" s="22"/>
       <c r="D29" s="34" t="s">
@@ -1489,7 +1675,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="30" spans="2:6" ht="15" x14ac:dyDescent="0.25">
+    <row r="30" spans="2:6" ht="14" x14ac:dyDescent="0.3">
       <c r="B30" s="23" t="s">
         <v>24</v>
       </c>
@@ -1502,30 +1688,30 @@
       </c>
       <c r="F30" s="23"/>
     </row>
-    <row r="31" spans="2:6" ht="15" x14ac:dyDescent="0.25">
+    <row r="31" spans="2:6" ht="14" x14ac:dyDescent="0.3">
       <c r="B31" s="31"/>
       <c r="C31" s="32"/>
       <c r="D31" s="33"/>
       <c r="E31" s="31"/>
       <c r="F31" s="31"/>
     </row>
-    <row r="32" spans="2:6" ht="12" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="33" spans="2:4" hidden="1" x14ac:dyDescent="0.2"/>
-    <row r="34" spans="2:4" ht="22.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B34" s="57" t="s">
+    <row r="32" spans="2:6" ht="12" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="33" spans="2:4" hidden="1" x14ac:dyDescent="0.25"/>
+    <row r="34" spans="2:4" ht="22.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B34" s="52" t="s">
         <v>46</v>
       </c>
-      <c r="C34" s="58"/>
-      <c r="D34" s="59"/>
-    </row>
-    <row r="35" spans="2:4" x14ac:dyDescent="0.2">
+      <c r="C34" s="53"/>
+      <c r="D34" s="54"/>
+    </row>
+    <row r="35" spans="2:4" ht="13" x14ac:dyDescent="0.3">
       <c r="B35" s="26"/>
-      <c r="C35" s="53" t="s">
+      <c r="C35" s="48" t="s">
         <v>32</v>
       </c>
-      <c r="D35" s="54"/>
-    </row>
-    <row r="36" spans="2:4" x14ac:dyDescent="0.2">
+      <c r="D35" s="49"/>
+    </row>
+    <row r="36" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B36" s="27" t="s">
         <v>33</v>
       </c>
@@ -1534,22 +1720,294 @@
       </c>
       <c r="D36" s="29"/>
     </row>
-    <row r="37" spans="2:4" x14ac:dyDescent="0.2">
+    <row r="37" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B37" s="30" t="s">
         <v>35</v>
       </c>
-      <c r="C37" s="55" t="s">
+      <c r="C37" s="50" t="s">
         <v>42</v>
       </c>
-      <c r="D37" s="56"/>
+      <c r="D37" s="51"/>
+    </row>
+    <row r="44" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B44" s="35" t="s">
+        <v>57</v>
+      </c>
+      <c r="C44" s="35"/>
+    </row>
+    <row r="45" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B45" s="3" t="s">
+        <v>49</v>
+      </c>
+      <c r="C45" s="3" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="46" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B46" s="3" t="s">
+        <v>56</v>
+      </c>
+      <c r="C46" s="3"/>
+    </row>
+    <row r="47" spans="2:4" ht="13" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B47" s="3" t="s">
+        <v>50</v>
+      </c>
+      <c r="C47" s="3" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="48" spans="2:4" ht="13.5" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B48" s="6" t="s">
+        <v>51</v>
+      </c>
+      <c r="C48" s="9" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="49" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B49" s="7">
+        <v>2</v>
+      </c>
+      <c r="C49" s="11" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="50" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B50" s="8"/>
+      <c r="C50" s="11" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="55" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B55" s="35" t="s">
+        <v>59</v>
+      </c>
+      <c r="C55" s="35"/>
+      <c r="D55" s="35"/>
+    </row>
+    <row r="56" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B56" s="3" t="s">
+        <v>49</v>
+      </c>
+      <c r="C56" s="69" t="s">
+        <v>3</v>
+      </c>
+      <c r="D56" s="70"/>
+    </row>
+    <row r="57" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B57" s="3" t="s">
+        <v>56</v>
+      </c>
+      <c r="C57" s="64"/>
+      <c r="D57" s="66"/>
+    </row>
+    <row r="58" spans="2:4" ht="13" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B58" s="3" t="s">
+        <v>50</v>
+      </c>
+      <c r="C58" s="64" t="s">
+        <v>54</v>
+      </c>
+      <c r="D58" s="66"/>
+    </row>
+    <row r="59" spans="2:4" ht="13.5" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B59" s="6" t="s">
+        <v>51</v>
+      </c>
+      <c r="C59" s="67" t="s">
+        <v>52</v>
+      </c>
+      <c r="D59" s="71"/>
+    </row>
+    <row r="60" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B60" s="7">
+        <v>2</v>
+      </c>
+      <c r="C60" s="11" t="s">
+        <v>55</v>
+      </c>
+      <c r="D60" s="11" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="61" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B61" s="8">
+        <v>2</v>
+      </c>
+      <c r="C61" s="11" t="s">
+        <v>55</v>
+      </c>
+      <c r="D61" s="11" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="65" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B65" s="35" t="s">
+        <v>58</v>
+      </c>
+      <c r="C65" s="35"/>
+      <c r="D65" s="35"/>
+      <c r="E65" s="35"/>
+    </row>
+    <row r="66" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B66" s="3" t="s">
+        <v>49</v>
+      </c>
+      <c r="C66" s="69" t="s">
+        <v>3</v>
+      </c>
+      <c r="D66" s="72"/>
+      <c r="E66" s="70"/>
+    </row>
+    <row r="67" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B67" s="3" t="s">
+        <v>56</v>
+      </c>
+      <c r="C67" s="64"/>
+      <c r="D67" s="65"/>
+      <c r="E67" s="66"/>
+    </row>
+    <row r="68" spans="2:5" ht="13" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B68" s="3" t="s">
+        <v>50</v>
+      </c>
+      <c r="C68" s="64" t="s">
+        <v>53</v>
+      </c>
+      <c r="D68" s="65"/>
+      <c r="E68" s="66"/>
+    </row>
+    <row r="69" spans="2:5" ht="13.5" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B69" s="6" t="s">
+        <v>51</v>
+      </c>
+      <c r="C69" s="67" t="s">
+        <v>52</v>
+      </c>
+      <c r="D69" s="68"/>
+      <c r="E69" s="68"/>
+    </row>
+    <row r="70" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B70" s="7">
+        <v>2</v>
+      </c>
+      <c r="C70" s="11" t="s">
+        <v>55</v>
+      </c>
+      <c r="D70" s="11" t="s">
+        <v>55</v>
+      </c>
+      <c r="E70" s="11" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="71" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B71" s="8"/>
+      <c r="C71" s="11" t="s">
+        <v>55</v>
+      </c>
+      <c r="D71" s="11" t="s">
+        <v>55</v>
+      </c>
+      <c r="E71" s="11" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="75" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B75" s="35" t="s">
+        <v>60</v>
+      </c>
+      <c r="C75" s="35"/>
+      <c r="D75" s="35"/>
+    </row>
+    <row r="76" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B76" s="3" t="s">
+        <v>49</v>
+      </c>
+      <c r="C76" s="69" t="s">
+        <v>3</v>
+      </c>
+      <c r="D76" s="70"/>
+    </row>
+    <row r="77" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B77" s="3" t="s">
+        <v>56</v>
+      </c>
+      <c r="C77" s="64"/>
+      <c r="D77" s="66"/>
+    </row>
+    <row r="78" spans="2:5" ht="13" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B78" s="3" t="s">
+        <v>50</v>
+      </c>
+      <c r="C78" s="64" t="s">
+        <v>53</v>
+      </c>
+      <c r="D78" s="66"/>
+    </row>
+    <row r="79" spans="2:5" ht="13.5" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B79" s="6" t="s">
+        <v>51</v>
+      </c>
+      <c r="C79" s="67" t="s">
+        <v>52</v>
+      </c>
+      <c r="D79" s="71"/>
+    </row>
+    <row r="80" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B80" s="73">
+        <v>2</v>
+      </c>
+      <c r="C80" s="11" t="s">
+        <v>55</v>
+      </c>
+      <c r="D80" s="11" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="81" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B81" s="74"/>
+      <c r="C81" s="11" t="s">
+        <v>55</v>
+      </c>
+      <c r="D81" s="11" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="82" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B82" s="75"/>
+      <c r="C82" s="11" t="s">
+        <v>55</v>
+      </c>
+      <c r="D82" s="11" t="s">
+        <v>55</v>
+      </c>
     </row>
   </sheetData>
-  <mergeCells count="24">
-    <mergeCell ref="B3:C3"/>
-    <mergeCell ref="K3:M3"/>
-    <mergeCell ref="K4:M4"/>
-    <mergeCell ref="B13:B14"/>
-    <mergeCell ref="B12:D12"/>
+  <mergeCells count="41">
+    <mergeCell ref="B80:B82"/>
+    <mergeCell ref="B75:D75"/>
+    <mergeCell ref="C76:D76"/>
+    <mergeCell ref="C77:D77"/>
+    <mergeCell ref="C78:D78"/>
+    <mergeCell ref="C79:D79"/>
+    <mergeCell ref="B44:C44"/>
+    <mergeCell ref="B55:D55"/>
+    <mergeCell ref="B65:E65"/>
+    <mergeCell ref="C66:E66"/>
+    <mergeCell ref="C67:E67"/>
+    <mergeCell ref="C68:E68"/>
+    <mergeCell ref="C69:E69"/>
+    <mergeCell ref="C56:D56"/>
+    <mergeCell ref="C57:D57"/>
+    <mergeCell ref="C58:D58"/>
+    <mergeCell ref="C59:D59"/>
+    <mergeCell ref="C15:D15"/>
+    <mergeCell ref="C16:D16"/>
+    <mergeCell ref="C17:D17"/>
+    <mergeCell ref="C18:D18"/>
+    <mergeCell ref="C19:D19"/>
     <mergeCell ref="B25:B26"/>
     <mergeCell ref="C25:C26"/>
     <mergeCell ref="C20:D20"/>
@@ -1559,11 +2017,11 @@
     <mergeCell ref="B23:F23"/>
     <mergeCell ref="D25:D26"/>
     <mergeCell ref="E25:F25"/>
-    <mergeCell ref="C15:D15"/>
-    <mergeCell ref="C16:D16"/>
-    <mergeCell ref="C17:D17"/>
-    <mergeCell ref="C18:D18"/>
-    <mergeCell ref="C19:D19"/>
+    <mergeCell ref="B3:C3"/>
+    <mergeCell ref="K3:M3"/>
+    <mergeCell ref="K4:M4"/>
+    <mergeCell ref="B13:B14"/>
+    <mergeCell ref="B12:D12"/>
     <mergeCell ref="K8:M8"/>
     <mergeCell ref="K9:M9"/>
     <mergeCell ref="K10:M10"/>
@@ -1571,5 +2029,6 @@
     <mergeCell ref="K12:M12"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>